<commit_message>
Add Login & Akun Saya
</commit_message>
<xml_diff>
--- a/Excel/user_data.xlsx
+++ b/Excel/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Katalon Studio\Tugas Automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED1E89A-ADEC-4C4F-B159-E11E48E6994F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4AC4AA-CAEF-4B9A-A9E8-0AA0A04CC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8627A078-35FE-4D02-9890-0F34478703D6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A42504B-0FFE-4C0A-97B3-4331FE924BCE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,13 +434,24 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3878F08A-9E1D-4F60-A906-5CC4FCAFBA50}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{3878F08A-9E1D-4F60-A906-5CC4FCAFBA50}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{6CC1FD15-0D0B-415A-A0C4-BDE3126E21B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>